<commit_message>
Ready for PR (5)
</commit_message>
<xml_diff>
--- a/results/raw/results.xlsx
+++ b/results/raw/results.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maxirmx/Projects/tebako-benchmarking/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\8.Projects\tebako-benchmarking\results\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{ECDF5B35-48B8-8447-A180-FB4743147925}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3473767C-1CFA-4502-9391-771C85538E8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11580" yWindow="5400" windowWidth="35860" windowHeight="17440" xr2:uid="{CC4E95A0-18F8-C345-87FB-74ABA326F855}"/>
+    <workbookView xWindow="2080" yWindow="2080" windowWidth="28890" windowHeight="18520" xr2:uid="{CC4E95A0-18F8-C345-87FB-74ABA326F855}"/>
   </bookViews>
   <sheets>
     <sheet name="Simple test (Hello, world)" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,6 +27,7 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
         <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -84,7 +85,7 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -102,7 +103,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="ru-RU"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -120,7 +121,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="1680" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -134,13 +135,8 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-GB"/>
-              <a:t>Comparison</a:t>
+              <a:t> Benchmarking for 'Hello, world" script</a:t>
             </a:r>
-            <a:r>
-              <a:rPr lang="en-GB" baseline="0"/>
-              <a:t> for 'Hello, world" script</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-GB"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -157,7 +153,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1680" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -169,7 +165,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-RU"/>
+          <a:endParaRPr lang="ru-RU"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -452,7 +448,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -465,14 +461,9 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-GB" sz="1100"/>
-                  <a:t>Number</a:t>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Number of repetitions</a:t>
                 </a:r>
-                <a:r>
-                  <a:rPr lang="en-GB" sz="1100" baseline="0"/>
-                  <a:t> of repetitions</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-GB" sz="1100"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -489,7 +480,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -501,7 +492,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-RU"/>
+              <a:endParaRPr lang="ru-RU"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -527,7 +518,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -539,7 +530,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-RU"/>
+            <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1858498064"/>
@@ -578,7 +569,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -591,7 +582,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-GB" sz="1100"/>
+                  <a:rPr lang="en-GB"/>
                   <a:t>Execution time (user + sys), seconds</a:t>
                 </a:r>
               </a:p>
@@ -610,7 +601,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -622,7 +613,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-RU"/>
+              <a:endParaRPr lang="ru-RU"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -642,7 +633,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -654,7 +645,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-RU"/>
+            <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="521009296"/>
@@ -684,7 +675,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr rtl="0">
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -696,7 +687,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-RU"/>
+            <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
       </c:dTable>
@@ -739,9 +730,9 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr/>
+        <a:defRPr sz="1400"/>
       </a:pPr>
-      <a:endParaRPr lang="en-RU"/>
+      <a:endParaRPr lang="ru-RU"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1299,15 +1290,15 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>12700</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>806450</xdr:colOff>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>101600</xdr:colOff>
-      <xdr:row>43</xdr:row>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>39</xdr:row>
       <xdr:rowOff>101600</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1337,9 +1328,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1377,7 +1368,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1483,7 +1474,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1635,18 +1626,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{011826E9-9A44-C042-A061-04C93FF74651}">
   <dimension ref="A3:L6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="25.33203125" customWidth="1"/>
     <col min="10" max="10" width="11.1640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B3" s="1">
         <v>1</v>
       </c>
@@ -1679,7 +1670,7 @@
       </c>
       <c r="L3" s="1"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -1714,7 +1705,7 @@
         <v>1759.48</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -1749,48 +1740,48 @@
         <v>1186.0899999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>2</v>
       </c>
       <c r="B6">
-        <f>B4/B3</f>
+        <f t="shared" ref="B6:K6" si="0">B4/B3</f>
         <v>0.03</v>
       </c>
       <c r="C6">
-        <f>C4/C3</f>
+        <f t="shared" si="0"/>
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="D6">
-        <f>D4/D3</f>
+        <f t="shared" si="0"/>
         <v>2.9999999999999997E-4</v>
       </c>
       <c r="E6">
-        <f>E4/E3</f>
+        <f t="shared" si="0"/>
         <v>2.9999999999999997E-5</v>
       </c>
       <c r="F6">
-        <f>F4/F3</f>
+        <f t="shared" si="0"/>
         <v>5.0000000000000004E-6</v>
       </c>
       <c r="G6">
-        <f>G4/G3</f>
+        <f t="shared" si="0"/>
         <v>1.9999999999999999E-6</v>
       </c>
       <c r="H6">
-        <f>H4/H3</f>
+        <f t="shared" si="0"/>
         <v>1.7800000000000001E-6</v>
       </c>
       <c r="I6">
-        <f>I4/I3</f>
+        <f t="shared" si="0"/>
         <v>1.748E-6</v>
       </c>
       <c r="J6">
-        <f>J4/J3</f>
+        <f t="shared" si="0"/>
         <v>1.7733E-6</v>
       </c>
       <c r="K6">
-        <f>K4/K3</f>
+        <f t="shared" si="0"/>
         <v>1.7594799999999999E-6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added coradoc Gem benchmarking (#3)
</commit_message>
<xml_diff>
--- a/results/raw/results.xlsx
+++ b/results/raw/results.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\8.Projects\tebako-benchmarking\results\raw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maxirmx/Projects/tebako-benchmarking/results/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3473767C-1CFA-4502-9391-771C85538E8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DDD90AF-49DA-AC44-93AE-C972C80B93C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2080" yWindow="2080" windowWidth="28890" windowHeight="18520" xr2:uid="{CC4E95A0-18F8-C345-87FB-74ABA326F855}"/>
+    <workbookView xWindow="2080" yWindow="2080" windowWidth="37580" windowHeight="18520" activeTab="1" xr2:uid="{CC4E95A0-18F8-C345-87FB-74ABA326F855}"/>
   </bookViews>
   <sheets>
     <sheet name="Simple test (Hello, world)" sheetId="1" r:id="rId1"/>
+    <sheet name="coradoc test" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,15 +37,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="2">
   <si>
     <t xml:space="preserve">Plain Ruby </t>
   </si>
   <si>
     <t>Tebako package</t>
-  </si>
-  <si>
-    <t>Plain Ruby weighted</t>
   </si>
 </sst>
 </file>
@@ -85,7 +83,7 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -103,7 +101,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="ru-RU"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -165,7 +163,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="ru-RU"/>
+          <a:endParaRPr lang="en-RU"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -492,7 +490,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="ru-RU"/>
+              <a:endParaRPr lang="en-RU"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -530,7 +528,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="ru-RU"/>
+            <a:endParaRPr lang="en-RU"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1858498064"/>
@@ -613,7 +611,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="ru-RU"/>
+              <a:endParaRPr lang="en-RU"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -645,7 +643,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="ru-RU"/>
+            <a:endParaRPr lang="en-RU"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="521009296"/>
@@ -687,7 +685,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="ru-RU"/>
+            <a:endParaRPr lang="en-RU"/>
           </a:p>
         </c:txPr>
       </c:dTable>
@@ -732,7 +730,601 @@
       <a:pPr>
         <a:defRPr sz="1400"/>
       </a:pPr>
-      <a:endParaRPr lang="ru-RU"/>
+      <a:endParaRPr lang="en-RU"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1680" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t> Benchmarking for coradoc script</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1680" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-RU"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'coradoc test'!$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Plain Ruby </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'coradoc test'!$B$3:$G$3</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'coradoc test'!$B$4:$G$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.49</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.57</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>45.34</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>219.05</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>452.48</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>871.05</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-AB77-574D-A3DB-A463D9C08B86}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'coradoc test'!$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Tebako package</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'coradoc test'!$B$3:$G$3</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'coradoc test'!$B$5:$G$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.04</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40.33</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>201.17</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>402.28</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>801.61</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-AB77-574D-A3DB-A463D9C08B86}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="521009296"/>
+        <c:axId val="1858498064"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="521009296"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Number of repetitions</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-RU"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="#,##0" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1858498064"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1858498064"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Execution time (user + sys), seconds</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-RU"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="521009296"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:dTable>
+        <c:showHorzBorder val="1"/>
+        <c:showVertBorder val="1"/>
+        <c:showOutline val="1"/>
+        <c:showKeys val="1"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr rtl="0">
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-RU"/>
+          </a:p>
+        </c:txPr>
+      </c:dTable>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1400"/>
+      </a:pPr>
+      <a:endParaRPr lang="en-RU"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -783,7 +1375,550 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -1292,13 +2427,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>806450</xdr:colOff>
-      <xdr:row>11</xdr:row>
+      <xdr:row>9</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
       <xdr:colOff>247650</xdr:colOff>
-      <xdr:row>39</xdr:row>
+      <xdr:row>37</xdr:row>
       <xdr:rowOff>101600</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1327,10 +2462,53 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>806450</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C7F014D9-73AE-2D42-BC48-924358147A72}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1368,7 +2546,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1474,7 +2652,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1624,20 +2802,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{011826E9-9A44-C042-A061-04C93FF74651}">
-  <dimension ref="A3:L6"/>
+  <dimension ref="A3:L5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="25.33203125" customWidth="1"/>
     <col min="10" max="10" width="11.1640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B3" s="1">
         <v>1</v>
       </c>
@@ -1670,7 +2848,7 @@
       </c>
       <c r="L3" s="1"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -1705,7 +2883,7 @@
         <v>1759.48</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -1740,49 +2918,97 @@
         <v>1186.0899999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6">
-        <f t="shared" ref="B6:K6" si="0">B4/B3</f>
-        <v>0.03</v>
-      </c>
-      <c r="C6">
-        <f t="shared" si="0"/>
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="D6">
-        <f t="shared" si="0"/>
-        <v>2.9999999999999997E-4</v>
-      </c>
-      <c r="E6">
-        <f t="shared" si="0"/>
-        <v>2.9999999999999997E-5</v>
-      </c>
-      <c r="F6">
-        <f t="shared" si="0"/>
-        <v>5.0000000000000004E-6</v>
-      </c>
-      <c r="G6">
-        <f t="shared" si="0"/>
-        <v>1.9999999999999999E-6</v>
-      </c>
-      <c r="H6">
-        <f t="shared" si="0"/>
-        <v>1.7800000000000001E-6</v>
-      </c>
-      <c r="I6">
-        <f t="shared" si="0"/>
-        <v>1.748E-6</v>
-      </c>
-      <c r="J6">
-        <f t="shared" si="0"/>
-        <v>1.7733E-6</v>
-      </c>
-      <c r="K6">
-        <f t="shared" si="0"/>
-        <v>1.7594799999999999E-6</v>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31A805AF-75BC-D948-96DC-630440D94538}">
+  <dimension ref="A3:M5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="25.33203125" customWidth="1"/>
+    <col min="11" max="11" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B3" s="1">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1">
+        <v>10</v>
+      </c>
+      <c r="D3" s="1">
+        <v>100</v>
+      </c>
+      <c r="E3" s="1">
+        <v>500</v>
+      </c>
+      <c r="F3" s="1">
+        <v>1000</v>
+      </c>
+      <c r="G3" s="1">
+        <v>2000</v>
+      </c>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4">
+        <v>0.49</v>
+      </c>
+      <c r="C4">
+        <v>4.57</v>
+      </c>
+      <c r="D4">
+        <v>45.34</v>
+      </c>
+      <c r="E4">
+        <v>219.05</v>
+      </c>
+      <c r="F4">
+        <v>452.48</v>
+      </c>
+      <c r="G4">
+        <v>871.05</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>0.5</v>
+      </c>
+      <c r="C5">
+        <v>4.04</v>
+      </c>
+      <c r="D5">
+        <v>40.33</v>
+      </c>
+      <c r="E5">
+        <v>201.17</v>
+      </c>
+      <c r="F5">
+        <v>402.28</v>
+      </c>
+      <c r="G5">
+        <v>801.61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added emf2svg benchmarking (#4)
</commit_message>
<xml_diff>
--- a/results/raw/results.xlsx
+++ b/results/raw/results.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maxirmx/Projects/tebako-benchmarking/results/raw/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\8.Projects\tebako-benchmarking\results\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DDD90AF-49DA-AC44-93AE-C972C80B93C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B13B25F-455E-4705-9065-5324FB44807C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2080" yWindow="2080" windowWidth="37580" windowHeight="18520" activeTab="1" xr2:uid="{CC4E95A0-18F8-C345-87FB-74ABA326F855}"/>
+    <workbookView xWindow="2080" yWindow="2080" windowWidth="32730" windowHeight="18520" xr2:uid="{CC4E95A0-18F8-C345-87FB-74ABA326F855}"/>
   </bookViews>
   <sheets>
     <sheet name="Simple test (Hello, world)" sheetId="1" r:id="rId1"/>
     <sheet name="coradoc test" sheetId="2" r:id="rId2"/>
+    <sheet name="emf2svg test" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="2">
   <si>
     <t xml:space="preserve">Plain Ruby </t>
   </si>
@@ -83,7 +84,7 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -101,7 +102,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="ru-RU"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -163,7 +164,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-RU"/>
+          <a:endParaRPr lang="ru-RU"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -490,7 +491,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-RU"/>
+              <a:endParaRPr lang="ru-RU"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -528,7 +529,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-RU"/>
+            <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1858498064"/>
@@ -611,7 +612,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-RU"/>
+              <a:endParaRPr lang="ru-RU"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -643,7 +644,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-RU"/>
+            <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="521009296"/>
@@ -685,7 +686,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-RU"/>
+            <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
       </c:dTable>
@@ -730,7 +731,7 @@
       <a:pPr>
         <a:defRPr sz="1400"/>
       </a:pPr>
-      <a:endParaRPr lang="en-RU"/>
+      <a:endParaRPr lang="ru-RU"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -744,7 +745,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="ru-RU"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -776,7 +777,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-GB"/>
-              <a:t> Benchmarking for coradoc script</a:t>
+              <a:t> Benchmarking for coradoc gem</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -806,7 +807,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-RU"/>
+          <a:endParaRPr lang="ru-RU"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1085,7 +1086,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-RU"/>
+              <a:endParaRPr lang="ru-RU"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1123,7 +1124,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-RU"/>
+            <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1858498064"/>
@@ -1136,6 +1137,7 @@
       <c:valAx>
         <c:axId val="1858498064"/>
         <c:scaling>
+          <c:logBase val="10"/>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -1205,7 +1207,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-RU"/>
+              <a:endParaRPr lang="ru-RU"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1237,7 +1239,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-RU"/>
+            <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="521009296"/>
@@ -1279,7 +1281,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-RU"/>
+            <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
       </c:dTable>
@@ -1324,7 +1326,638 @@
       <a:pPr>
         <a:defRPr sz="1400"/>
       </a:pPr>
-      <a:endParaRPr lang="en-RU"/>
+      <a:endParaRPr lang="ru-RU"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="ru-RU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1680" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t> Benchmarking for emf2svg gem</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1680" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ru-RU"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'emf2svg test'!$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Plain Ruby </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'emf2svg test'!$B$3:$J$3</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>500000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'emf2svg test'!$B$4:$J$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.06</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.17</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.26</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12.23</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>60.65</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>121.24</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>241.99</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-DD2E-AC42-8FBB-77921B802420}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'emf2svg test'!$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Tebako package</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'emf2svg test'!$B$3:$J$3</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>500000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'emf2svg test'!$B$5:$J$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.09</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.11</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.12</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.23</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.31</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11.98</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>59.4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>119.28</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>237.81</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-DD2E-AC42-8FBB-77921B802420}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="521009296"/>
+        <c:axId val="1858498064"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="521009296"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Number of repetitions</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="ru-RU"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="#,##0" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1858498064"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1858498064"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Execution time (user + sys), seconds</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="ru-RU"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="521009296"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:dTable>
+        <c:showHorzBorder val="1"/>
+        <c:showVertBorder val="1"/>
+        <c:showOutline val="1"/>
+        <c:showKeys val="1"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr rtl="0">
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+      </c:dTable>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1400"/>
+      </a:pPr>
+      <a:endParaRPr lang="ru-RU"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1415,6 +2048,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
@@ -1919,6 +2592,509 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2505,10 +3681,53 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>806450</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DBE7F154-D269-4043-A18E-B65A40A9AD1F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2546,7 +3765,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2652,7 +3871,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2804,18 +4023,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{011826E9-9A44-C042-A061-04C93FF74651}">
   <dimension ref="A3:L5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="25.33203125" customWidth="1"/>
     <col min="10" max="10" width="11.1640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B3" s="1">
         <v>1</v>
       </c>
@@ -2848,7 +4067,7 @@
       </c>
       <c r="L3" s="1"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -2883,7 +4102,7 @@
         <v>1759.48</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -2928,18 +4147,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31A805AF-75BC-D948-96DC-630440D94538}">
   <dimension ref="A3:M5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="25.33203125" customWidth="1"/>
     <col min="11" max="11" width="11.1640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B3" s="1">
         <v>1</v>
       </c>
@@ -2965,7 +4184,7 @@
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -2988,7 +4207,7 @@
         <v>871.05</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -3009,6 +4228,124 @@
       </c>
       <c r="G5">
         <v>801.61</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DCA4F36-FE5D-C545-A7DB-A83B6D4CDF89}">
+  <dimension ref="A3:N5"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="25.33203125" customWidth="1"/>
+    <col min="12" max="12" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B3" s="1">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1">
+        <v>10</v>
+      </c>
+      <c r="D3" s="1">
+        <v>100</v>
+      </c>
+      <c r="E3" s="1">
+        <v>1000</v>
+      </c>
+      <c r="F3" s="1">
+        <v>10000</v>
+      </c>
+      <c r="G3" s="1">
+        <v>100000</v>
+      </c>
+      <c r="H3" s="1">
+        <v>500000</v>
+      </c>
+      <c r="I3" s="1">
+        <v>1000000</v>
+      </c>
+      <c r="J3" s="1">
+        <v>2000000</v>
+      </c>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4">
+        <v>0.05</v>
+      </c>
+      <c r="C4">
+        <v>0.05</v>
+      </c>
+      <c r="D4">
+        <v>0.06</v>
+      </c>
+      <c r="E4">
+        <v>0.17</v>
+      </c>
+      <c r="F4">
+        <v>1.26</v>
+      </c>
+      <c r="G4">
+        <v>12.23</v>
+      </c>
+      <c r="H4">
+        <v>60.65</v>
+      </c>
+      <c r="I4">
+        <v>121.24</v>
+      </c>
+      <c r="J4">
+        <v>241.99</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>0.09</v>
+      </c>
+      <c r="C5">
+        <v>0.11</v>
+      </c>
+      <c r="D5">
+        <v>0.12</v>
+      </c>
+      <c r="E5">
+        <v>0.23</v>
+      </c>
+      <c r="F5">
+        <v>1.31</v>
+      </c>
+      <c r="G5">
+        <v>11.98</v>
+      </c>
+      <c r="H5">
+        <v>59.4</v>
+      </c>
+      <c r="I5">
+        <v>119.28</v>
+      </c>
+      <c r="J5">
+        <v>237.81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added vectory gem benchmarking
</commit_message>
<xml_diff>
--- a/results/raw/results.xlsx
+++ b/results/raw/results.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\8.Projects\tebako-benchmarking\results\raw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maxirmx/Projects/tebako-benchmarking/results/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B13B25F-455E-4705-9065-5324FB44807C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3D9FCCE-AED9-944D-B8AA-1458DDDB086D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2080" yWindow="2080" windowWidth="32730" windowHeight="18520" xr2:uid="{CC4E95A0-18F8-C345-87FB-74ABA326F855}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="26380" xr2:uid="{CC4E95A0-18F8-C345-87FB-74ABA326F855}"/>
   </bookViews>
   <sheets>
-    <sheet name="Simple test (Hello, world)" sheetId="1" r:id="rId1"/>
-    <sheet name="coradoc test" sheetId="2" r:id="rId2"/>
-    <sheet name="emf2svg test" sheetId="3" r:id="rId3"/>
+    <sheet name="Simple script" sheetId="1" r:id="rId1"/>
+    <sheet name="coradoc gem" sheetId="2" r:id="rId2"/>
+    <sheet name="emf2svg gem" sheetId="3" r:id="rId3"/>
+    <sheet name="vectory gem" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="2">
   <si>
     <t xml:space="preserve">Plain Ruby </t>
   </si>
@@ -84,7 +85,7 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -102,7 +103,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="ru-RU"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -164,7 +165,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="ru-RU"/>
+          <a:endParaRPr lang="en-RU"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -179,7 +180,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Simple test (Hello, world)'!$A$4</c:f>
+              <c:f>'Simple script'!$A$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -214,7 +215,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Simple test (Hello, world)'!$B$3:$K$3</c:f>
+              <c:f>'Simple script'!$B$3:$K$3</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="10"/>
@@ -253,7 +254,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Simple test (Hello, world)'!$B$4:$K$4</c:f>
+              <c:f>'Simple script'!$B$4:$K$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -302,7 +303,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Simple test (Hello, world)'!$A$5</c:f>
+              <c:f>'Simple script'!$A$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -337,7 +338,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Simple test (Hello, world)'!$B$3:$K$3</c:f>
+              <c:f>'Simple script'!$B$3:$K$3</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="10"/>
@@ -376,7 +377,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Simple test (Hello, world)'!$B$5:$K$5</c:f>
+              <c:f>'Simple script'!$B$5:$K$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -491,7 +492,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="ru-RU"/>
+              <a:endParaRPr lang="en-RU"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -529,7 +530,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="ru-RU"/>
+            <a:endParaRPr lang="en-RU"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1858498064"/>
@@ -612,7 +613,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="ru-RU"/>
+              <a:endParaRPr lang="en-RU"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -644,7 +645,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="ru-RU"/>
+            <a:endParaRPr lang="en-RU"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="521009296"/>
@@ -686,7 +687,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="ru-RU"/>
+            <a:endParaRPr lang="en-RU"/>
           </a:p>
         </c:txPr>
       </c:dTable>
@@ -731,7 +732,7 @@
       <a:pPr>
         <a:defRPr sz="1400"/>
       </a:pPr>
-      <a:endParaRPr lang="ru-RU"/>
+      <a:endParaRPr lang="en-RU"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -745,7 +746,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="ru-RU"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -807,7 +808,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="ru-RU"/>
+          <a:endParaRPr lang="en-RU"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -822,7 +823,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'coradoc test'!$A$4</c:f>
+              <c:f>'coradoc gem'!$A$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -857,54 +858,60 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'coradoc test'!$B$3:$G$3</c:f>
+              <c:f>'coradoc gem'!$B$3:$H$3</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>100</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>500</c:v>
+                  <c:v>64</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1000</c:v>
+                  <c:v>256</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2000</c:v>
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4096</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'coradoc test'!$B$4:$G$4</c:f>
+              <c:f>'coradoc gem'!$B$4:$H$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0.49</c:v>
+                  <c:v>0.48</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.57</c:v>
+                  <c:v>1.77</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>45.34</c:v>
+                  <c:v>6.97</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>219.05</c:v>
+                  <c:v>26.24</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>452.48</c:v>
+                  <c:v>102.84</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>871.05</c:v>
+                  <c:v>414.51</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1643.93</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -921,7 +928,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'coradoc test'!$A$5</c:f>
+              <c:f>'coradoc gem'!$A$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -956,54 +963,60 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'coradoc test'!$B$3:$G$3</c:f>
+              <c:f>'coradoc gem'!$B$3:$H$3</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>100</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>500</c:v>
+                  <c:v>64</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1000</c:v>
+                  <c:v>256</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2000</c:v>
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4096</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'coradoc test'!$B$5:$G$5</c:f>
+              <c:f>'coradoc gem'!$B$5:$H$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0.5</c:v>
+                  <c:v>0.52</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.04</c:v>
+                  <c:v>1.71</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>40.33</c:v>
+                  <c:v>6.45</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>201.17</c:v>
+                  <c:v>25.84</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>402.28</c:v>
+                  <c:v>103.6</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>801.61</c:v>
+                  <c:v>420.7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1650.12</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1086,7 +1099,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="ru-RU"/>
+              <a:endParaRPr lang="en-RU"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1124,7 +1137,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="ru-RU"/>
+            <a:endParaRPr lang="en-RU"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1858498064"/>
@@ -1207,7 +1220,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="ru-RU"/>
+              <a:endParaRPr lang="en-RU"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1239,7 +1252,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="ru-RU"/>
+            <a:endParaRPr lang="en-RU"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="521009296"/>
@@ -1281,7 +1294,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="ru-RU"/>
+            <a:endParaRPr lang="en-RU"/>
           </a:p>
         </c:txPr>
       </c:dTable>
@@ -1326,7 +1339,7 @@
       <a:pPr>
         <a:defRPr sz="1400"/>
       </a:pPr>
-      <a:endParaRPr lang="ru-RU"/>
+      <a:endParaRPr lang="en-RU"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1340,7 +1353,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="ru-RU"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1402,7 +1415,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="ru-RU"/>
+          <a:endParaRPr lang="en-RU"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1417,7 +1430,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'emf2svg test'!$A$4</c:f>
+              <c:f>'emf2svg gem'!$A$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1452,10 +1465,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'emf2svg test'!$B$3:$J$3</c:f>
+              <c:f>'emf2svg gem'!$B$3:$H$3</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -1475,23 +1488,17 @@
                   <c:v>100000</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>500000</c:v>
-                </c:pt>
-                <c:pt idx="7">
                   <c:v>1000000</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>2000000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'emf2svg test'!$B$4:$J$4</c:f>
+              <c:f>'emf2svg gem'!$B$4:$H$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>0.05</c:v>
                 </c:pt>
@@ -1511,13 +1518,7 @@
                   <c:v>12.23</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>60.65</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>121.24</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>241.99</c:v>
+                  <c:v>120.81</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1534,7 +1535,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'emf2svg test'!$A$5</c:f>
+              <c:f>'emf2svg gem'!$A$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1569,10 +1570,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'emf2svg test'!$B$3:$J$3</c:f>
+              <c:f>'emf2svg gem'!$B$3:$H$3</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -1592,31 +1593,25 @@
                   <c:v>100000</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>500000</c:v>
-                </c:pt>
-                <c:pt idx="7">
                   <c:v>1000000</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>2000000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'emf2svg test'!$B$5:$J$5</c:f>
+              <c:f>'emf2svg gem'!$B$5:$H$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0.09</c:v>
+                  <c:v>0.11</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.11</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.12</c:v>
+                  <c:v>0.11</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0.23</c:v>
@@ -1625,16 +1620,10 @@
                   <c:v>1.31</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>11.98</c:v>
+                  <c:v>12.1</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>59.4</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>119.28</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>237.81</c:v>
+                  <c:v>118.93</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1717,7 +1706,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="ru-RU"/>
+              <a:endParaRPr lang="en-RU"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1755,7 +1744,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="ru-RU"/>
+            <a:endParaRPr lang="en-RU"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1858498064"/>
@@ -1838,7 +1827,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="ru-RU"/>
+              <a:endParaRPr lang="en-RU"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1870,7 +1859,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="ru-RU"/>
+            <a:endParaRPr lang="en-RU"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="521009296"/>
@@ -1912,7 +1901,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="ru-RU"/>
+            <a:endParaRPr lang="en-RU"/>
           </a:p>
         </c:txPr>
       </c:dTable>
@@ -1957,7 +1946,614 @@
       <a:pPr>
         <a:defRPr sz="1400"/>
       </a:pPr>
-      <a:endParaRPr lang="ru-RU"/>
+      <a:endParaRPr lang="en-RU"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1680" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t> Benchmarking for vectory gem</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1680" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-RU"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'vectory gem'!$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Plain Ruby </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'vectory gem'!$B$3:$H$3</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'vectory gem'!$B$4:$H$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.09</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.44</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.75</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>37.159999999999997</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>373.72</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D1C8-B946-9EA9-9FBEFFCDD148}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'vectory gem'!$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Tebako package</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'vectory gem'!$B$3:$H$3</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'vectory gem'!$B$5:$H$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.12</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.12</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.16</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.48</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.88</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>38.03</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>375.77</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-D1C8-B946-9EA9-9FBEFFCDD148}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="521009296"/>
+        <c:axId val="1858498064"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="521009296"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Number of repetitions</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-RU"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="#,##0" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1858498064"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1858498064"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Execution time (user + sys), seconds</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-RU"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="521009296"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:dTable>
+        <c:showHorzBorder val="1"/>
+        <c:showVertBorder val="1"/>
+        <c:showOutline val="1"/>
+        <c:showKeys val="1"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr rtl="0">
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-RU"/>
+          </a:p>
+        </c:txPr>
+      </c:dTable>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1400"/>
+      </a:pPr>
+      <a:endParaRPr lang="en-RU"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2088,6 +2684,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
@@ -3095,6 +3731,509 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -3691,7 +4830,7 @@
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
+      <xdr:col>20</xdr:col>
       <xdr:colOff>247650</xdr:colOff>
       <xdr:row>37</xdr:row>
       <xdr:rowOff>101600</xdr:rowOff>
@@ -3724,10 +4863,53 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>806450</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BF5D5B59-F44A-6D4B-9FC6-BC06E4B77AD9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -3765,7 +4947,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -3871,7 +5053,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -4024,17 +5206,17 @@
   <dimension ref="A3:L5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD6"/>
+      <selection activeCell="C57" sqref="C57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="25.33203125" customWidth="1"/>
     <col min="10" max="10" width="11.1640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B3" s="1">
         <v>1</v>
       </c>
@@ -4067,7 +5249,7 @@
       </c>
       <c r="L3" s="1"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -4102,7 +5284,7 @@
         <v>1759.48</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -4148,86 +5330,94 @@
   <dimension ref="A3:M5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="C62" sqref="C62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="25.33203125" customWidth="1"/>
     <col min="11" max="11" width="11.1640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B3" s="1">
         <v>1</v>
       </c>
       <c r="C3" s="1">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D3" s="1">
-        <v>100</v>
+        <v>16</v>
       </c>
       <c r="E3" s="1">
-        <v>500</v>
+        <v>64</v>
       </c>
       <c r="F3" s="1">
-        <v>1000</v>
+        <v>256</v>
       </c>
       <c r="G3" s="1">
-        <v>2000</v>
-      </c>
-      <c r="H3" s="1"/>
+        <v>1024</v>
+      </c>
+      <c r="H3" s="1">
+        <v>4096</v>
+      </c>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>0</v>
       </c>
       <c r="B4">
-        <v>0.49</v>
+        <v>0.48</v>
       </c>
       <c r="C4">
-        <v>4.57</v>
+        <v>1.77</v>
       </c>
       <c r="D4">
-        <v>45.34</v>
+        <v>6.97</v>
       </c>
       <c r="E4">
-        <v>219.05</v>
+        <v>26.24</v>
       </c>
       <c r="F4">
-        <v>452.48</v>
+        <v>102.84</v>
       </c>
       <c r="G4">
-        <v>871.05</v>
+        <v>414.51</v>
+      </c>
+      <c r="H4">
+        <v>1643.93</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>1</v>
       </c>
       <c r="B5">
-        <v>0.5</v>
+        <v>0.52</v>
       </c>
       <c r="C5">
-        <v>4.04</v>
+        <v>1.71</v>
       </c>
       <c r="D5">
-        <v>40.33</v>
+        <v>6.45</v>
       </c>
       <c r="E5">
-        <v>201.17</v>
+        <v>25.84</v>
       </c>
       <c r="F5">
-        <v>402.28</v>
+        <v>103.6</v>
       </c>
       <c r="G5">
-        <v>801.61</v>
+        <v>420.7</v>
+      </c>
+      <c r="H5">
+        <v>1650.12</v>
       </c>
     </row>
   </sheetData>
@@ -4238,20 +5428,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DCA4F36-FE5D-C545-A7DB-A83B6D4CDF89}">
-  <dimension ref="A3:N5"/>
+  <dimension ref="A3:L5"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView zoomScale="150" workbookViewId="0">
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="25.33203125" customWidth="1"/>
-    <col min="12" max="12" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B3" s="1">
         <v>1</v>
       </c>
@@ -4271,20 +5461,14 @@
         <v>100000</v>
       </c>
       <c r="H3" s="1">
-        <v>500000</v>
-      </c>
-      <c r="I3" s="1">
         <v>1000000</v>
       </c>
-      <c r="J3" s="1">
-        <v>2000000</v>
-      </c>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
-      <c r="M3" s="1"/>
-      <c r="N3" s="1"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -4307,27 +5491,21 @@
         <v>12.23</v>
       </c>
       <c r="H4">
-        <v>60.65</v>
-      </c>
-      <c r="I4">
-        <v>121.24</v>
-      </c>
-      <c r="J4">
-        <v>241.99</v>
+        <v>120.81</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>1</v>
       </c>
       <c r="B5">
-        <v>0.09</v>
+        <v>0.11</v>
       </c>
       <c r="C5">
         <v>0.11</v>
       </c>
       <c r="D5">
-        <v>0.12</v>
+        <v>0.11</v>
       </c>
       <c r="E5">
         <v>0.23</v>
@@ -4336,16 +5514,110 @@
         <v>1.31</v>
       </c>
       <c r="G5">
-        <v>11.98</v>
+        <v>12.1</v>
       </c>
       <c r="H5">
-        <v>59.4</v>
-      </c>
-      <c r="I5">
-        <v>119.28</v>
-      </c>
-      <c r="J5">
-        <v>237.81</v>
+        <v>118.93</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{832F9567-5372-FC45-867D-7249C5F9991D}">
+  <dimension ref="A3:L5"/>
+  <sheetViews>
+    <sheetView zoomScale="150" workbookViewId="0">
+      <selection activeCell="E42" sqref="E42"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="25.33203125" customWidth="1"/>
+    <col min="10" max="10" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B3" s="1">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1">
+        <v>10</v>
+      </c>
+      <c r="D3" s="1">
+        <v>100</v>
+      </c>
+      <c r="E3" s="1">
+        <v>1000</v>
+      </c>
+      <c r="F3" s="1">
+        <v>10000</v>
+      </c>
+      <c r="G3" s="1">
+        <v>100000</v>
+      </c>
+      <c r="H3" s="1">
+        <v>1000000</v>
+      </c>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4">
+        <v>0.05</v>
+      </c>
+      <c r="C4">
+        <v>0.05</v>
+      </c>
+      <c r="D4">
+        <v>0.09</v>
+      </c>
+      <c r="E4">
+        <v>0.44</v>
+      </c>
+      <c r="F4">
+        <v>3.75</v>
+      </c>
+      <c r="G4">
+        <v>37.159999999999997</v>
+      </c>
+      <c r="H4">
+        <v>373.72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>0.12</v>
+      </c>
+      <c r="C5">
+        <v>0.12</v>
+      </c>
+      <c r="D5">
+        <v>0.16</v>
+      </c>
+      <c r="E5">
+        <v>0.48</v>
+      </c>
+      <c r="F5">
+        <v>3.88</v>
+      </c>
+      <c r="G5">
+        <v>38.03</v>
+      </c>
+      <c r="H5">
+        <v>375.77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Documented vectory gem benchmarking results (#5)
</commit_message>
<xml_diff>
--- a/results/raw/results.xlsx
+++ b/results/raw/results.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\8.Projects\tebako-benchmarking\results\raw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maxirmx/Projects/tebako-benchmarking/results/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B13B25F-455E-4705-9065-5324FB44807C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3D9FCCE-AED9-944D-B8AA-1458DDDB086D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2080" yWindow="2080" windowWidth="32730" windowHeight="18520" xr2:uid="{CC4E95A0-18F8-C345-87FB-74ABA326F855}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="26380" xr2:uid="{CC4E95A0-18F8-C345-87FB-74ABA326F855}"/>
   </bookViews>
   <sheets>
-    <sheet name="Simple test (Hello, world)" sheetId="1" r:id="rId1"/>
-    <sheet name="coradoc test" sheetId="2" r:id="rId2"/>
-    <sheet name="emf2svg test" sheetId="3" r:id="rId3"/>
+    <sheet name="Simple script" sheetId="1" r:id="rId1"/>
+    <sheet name="coradoc gem" sheetId="2" r:id="rId2"/>
+    <sheet name="emf2svg gem" sheetId="3" r:id="rId3"/>
+    <sheet name="vectory gem" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="2">
   <si>
     <t xml:space="preserve">Plain Ruby </t>
   </si>
@@ -84,7 +85,7 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -102,7 +103,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="ru-RU"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -164,7 +165,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="ru-RU"/>
+          <a:endParaRPr lang="en-RU"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -179,7 +180,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Simple test (Hello, world)'!$A$4</c:f>
+              <c:f>'Simple script'!$A$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -214,7 +215,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Simple test (Hello, world)'!$B$3:$K$3</c:f>
+              <c:f>'Simple script'!$B$3:$K$3</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="10"/>
@@ -253,7 +254,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Simple test (Hello, world)'!$B$4:$K$4</c:f>
+              <c:f>'Simple script'!$B$4:$K$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -302,7 +303,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Simple test (Hello, world)'!$A$5</c:f>
+              <c:f>'Simple script'!$A$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -337,7 +338,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Simple test (Hello, world)'!$B$3:$K$3</c:f>
+              <c:f>'Simple script'!$B$3:$K$3</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="10"/>
@@ -376,7 +377,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Simple test (Hello, world)'!$B$5:$K$5</c:f>
+              <c:f>'Simple script'!$B$5:$K$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -491,7 +492,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="ru-RU"/>
+              <a:endParaRPr lang="en-RU"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -529,7 +530,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="ru-RU"/>
+            <a:endParaRPr lang="en-RU"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1858498064"/>
@@ -612,7 +613,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="ru-RU"/>
+              <a:endParaRPr lang="en-RU"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -644,7 +645,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="ru-RU"/>
+            <a:endParaRPr lang="en-RU"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="521009296"/>
@@ -686,7 +687,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="ru-RU"/>
+            <a:endParaRPr lang="en-RU"/>
           </a:p>
         </c:txPr>
       </c:dTable>
@@ -731,7 +732,7 @@
       <a:pPr>
         <a:defRPr sz="1400"/>
       </a:pPr>
-      <a:endParaRPr lang="ru-RU"/>
+      <a:endParaRPr lang="en-RU"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -745,7 +746,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="ru-RU"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -807,7 +808,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="ru-RU"/>
+          <a:endParaRPr lang="en-RU"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -822,7 +823,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'coradoc test'!$A$4</c:f>
+              <c:f>'coradoc gem'!$A$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -857,54 +858,60 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'coradoc test'!$B$3:$G$3</c:f>
+              <c:f>'coradoc gem'!$B$3:$H$3</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>100</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>500</c:v>
+                  <c:v>64</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1000</c:v>
+                  <c:v>256</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2000</c:v>
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4096</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'coradoc test'!$B$4:$G$4</c:f>
+              <c:f>'coradoc gem'!$B$4:$H$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0.49</c:v>
+                  <c:v>0.48</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.57</c:v>
+                  <c:v>1.77</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>45.34</c:v>
+                  <c:v>6.97</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>219.05</c:v>
+                  <c:v>26.24</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>452.48</c:v>
+                  <c:v>102.84</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>871.05</c:v>
+                  <c:v>414.51</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1643.93</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -921,7 +928,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'coradoc test'!$A$5</c:f>
+              <c:f>'coradoc gem'!$A$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -956,54 +963,60 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'coradoc test'!$B$3:$G$3</c:f>
+              <c:f>'coradoc gem'!$B$3:$H$3</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>100</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>500</c:v>
+                  <c:v>64</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1000</c:v>
+                  <c:v>256</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2000</c:v>
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4096</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'coradoc test'!$B$5:$G$5</c:f>
+              <c:f>'coradoc gem'!$B$5:$H$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0.5</c:v>
+                  <c:v>0.52</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.04</c:v>
+                  <c:v>1.71</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>40.33</c:v>
+                  <c:v>6.45</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>201.17</c:v>
+                  <c:v>25.84</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>402.28</c:v>
+                  <c:v>103.6</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>801.61</c:v>
+                  <c:v>420.7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1650.12</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1086,7 +1099,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="ru-RU"/>
+              <a:endParaRPr lang="en-RU"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1124,7 +1137,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="ru-RU"/>
+            <a:endParaRPr lang="en-RU"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1858498064"/>
@@ -1207,7 +1220,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="ru-RU"/>
+              <a:endParaRPr lang="en-RU"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1239,7 +1252,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="ru-RU"/>
+            <a:endParaRPr lang="en-RU"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="521009296"/>
@@ -1281,7 +1294,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="ru-RU"/>
+            <a:endParaRPr lang="en-RU"/>
           </a:p>
         </c:txPr>
       </c:dTable>
@@ -1326,7 +1339,7 @@
       <a:pPr>
         <a:defRPr sz="1400"/>
       </a:pPr>
-      <a:endParaRPr lang="ru-RU"/>
+      <a:endParaRPr lang="en-RU"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1340,7 +1353,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="ru-RU"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1402,7 +1415,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="ru-RU"/>
+          <a:endParaRPr lang="en-RU"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1417,7 +1430,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'emf2svg test'!$A$4</c:f>
+              <c:f>'emf2svg gem'!$A$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1452,10 +1465,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'emf2svg test'!$B$3:$J$3</c:f>
+              <c:f>'emf2svg gem'!$B$3:$H$3</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -1475,23 +1488,17 @@
                   <c:v>100000</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>500000</c:v>
-                </c:pt>
-                <c:pt idx="7">
                   <c:v>1000000</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>2000000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'emf2svg test'!$B$4:$J$4</c:f>
+              <c:f>'emf2svg gem'!$B$4:$H$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>0.05</c:v>
                 </c:pt>
@@ -1511,13 +1518,7 @@
                   <c:v>12.23</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>60.65</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>121.24</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>241.99</c:v>
+                  <c:v>120.81</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1534,7 +1535,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'emf2svg test'!$A$5</c:f>
+              <c:f>'emf2svg gem'!$A$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1569,10 +1570,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'emf2svg test'!$B$3:$J$3</c:f>
+              <c:f>'emf2svg gem'!$B$3:$H$3</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -1592,31 +1593,25 @@
                   <c:v>100000</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>500000</c:v>
-                </c:pt>
-                <c:pt idx="7">
                   <c:v>1000000</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>2000000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'emf2svg test'!$B$5:$J$5</c:f>
+              <c:f>'emf2svg gem'!$B$5:$H$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0.09</c:v>
+                  <c:v>0.11</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.11</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.12</c:v>
+                  <c:v>0.11</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0.23</c:v>
@@ -1625,16 +1620,10 @@
                   <c:v>1.31</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>11.98</c:v>
+                  <c:v>12.1</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>59.4</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>119.28</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>237.81</c:v>
+                  <c:v>118.93</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1717,7 +1706,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="ru-RU"/>
+              <a:endParaRPr lang="en-RU"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1755,7 +1744,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="ru-RU"/>
+            <a:endParaRPr lang="en-RU"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1858498064"/>
@@ -1838,7 +1827,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="ru-RU"/>
+              <a:endParaRPr lang="en-RU"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1870,7 +1859,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="ru-RU"/>
+            <a:endParaRPr lang="en-RU"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="521009296"/>
@@ -1912,7 +1901,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="ru-RU"/>
+            <a:endParaRPr lang="en-RU"/>
           </a:p>
         </c:txPr>
       </c:dTable>
@@ -1957,7 +1946,614 @@
       <a:pPr>
         <a:defRPr sz="1400"/>
       </a:pPr>
-      <a:endParaRPr lang="ru-RU"/>
+      <a:endParaRPr lang="en-RU"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1680" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t> Benchmarking for vectory gem</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1680" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-RU"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'vectory gem'!$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Plain Ruby </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'vectory gem'!$B$3:$H$3</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'vectory gem'!$B$4:$H$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.09</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.44</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.75</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>37.159999999999997</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>373.72</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D1C8-B946-9EA9-9FBEFFCDD148}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'vectory gem'!$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Tebako package</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'vectory gem'!$B$3:$H$3</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'vectory gem'!$B$5:$H$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.12</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.12</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.16</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.48</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.88</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>38.03</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>375.77</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-D1C8-B946-9EA9-9FBEFFCDD148}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="521009296"/>
+        <c:axId val="1858498064"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="521009296"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Number of repetitions</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-RU"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="#,##0" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1858498064"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1858498064"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Execution time (user + sys), seconds</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-RU"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="521009296"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:dTable>
+        <c:showHorzBorder val="1"/>
+        <c:showVertBorder val="1"/>
+        <c:showOutline val="1"/>
+        <c:showKeys val="1"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr rtl="0">
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-RU"/>
+          </a:p>
+        </c:txPr>
+      </c:dTable>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1400"/>
+      </a:pPr>
+      <a:endParaRPr lang="en-RU"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2088,6 +2684,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
@@ -3095,6 +3731,509 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -3691,7 +4830,7 @@
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
+      <xdr:col>20</xdr:col>
       <xdr:colOff>247650</xdr:colOff>
       <xdr:row>37</xdr:row>
       <xdr:rowOff>101600</xdr:rowOff>
@@ -3724,10 +4863,53 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>806450</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BF5D5B59-F44A-6D4B-9FC6-BC06E4B77AD9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -3765,7 +4947,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -3871,7 +5053,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -4024,17 +5206,17 @@
   <dimension ref="A3:L5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD6"/>
+      <selection activeCell="C57" sqref="C57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="25.33203125" customWidth="1"/>
     <col min="10" max="10" width="11.1640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B3" s="1">
         <v>1</v>
       </c>
@@ -4067,7 +5249,7 @@
       </c>
       <c r="L3" s="1"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -4102,7 +5284,7 @@
         <v>1759.48</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -4148,86 +5330,94 @@
   <dimension ref="A3:M5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="C62" sqref="C62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="25.33203125" customWidth="1"/>
     <col min="11" max="11" width="11.1640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B3" s="1">
         <v>1</v>
       </c>
       <c r="C3" s="1">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D3" s="1">
-        <v>100</v>
+        <v>16</v>
       </c>
       <c r="E3" s="1">
-        <v>500</v>
+        <v>64</v>
       </c>
       <c r="F3" s="1">
-        <v>1000</v>
+        <v>256</v>
       </c>
       <c r="G3" s="1">
-        <v>2000</v>
-      </c>
-      <c r="H3" s="1"/>
+        <v>1024</v>
+      </c>
+      <c r="H3" s="1">
+        <v>4096</v>
+      </c>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>0</v>
       </c>
       <c r="B4">
-        <v>0.49</v>
+        <v>0.48</v>
       </c>
       <c r="C4">
-        <v>4.57</v>
+        <v>1.77</v>
       </c>
       <c r="D4">
-        <v>45.34</v>
+        <v>6.97</v>
       </c>
       <c r="E4">
-        <v>219.05</v>
+        <v>26.24</v>
       </c>
       <c r="F4">
-        <v>452.48</v>
+        <v>102.84</v>
       </c>
       <c r="G4">
-        <v>871.05</v>
+        <v>414.51</v>
+      </c>
+      <c r="H4">
+        <v>1643.93</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>1</v>
       </c>
       <c r="B5">
-        <v>0.5</v>
+        <v>0.52</v>
       </c>
       <c r="C5">
-        <v>4.04</v>
+        <v>1.71</v>
       </c>
       <c r="D5">
-        <v>40.33</v>
+        <v>6.45</v>
       </c>
       <c r="E5">
-        <v>201.17</v>
+        <v>25.84</v>
       </c>
       <c r="F5">
-        <v>402.28</v>
+        <v>103.6</v>
       </c>
       <c r="G5">
-        <v>801.61</v>
+        <v>420.7</v>
+      </c>
+      <c r="H5">
+        <v>1650.12</v>
       </c>
     </row>
   </sheetData>
@@ -4238,20 +5428,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DCA4F36-FE5D-C545-A7DB-A83B6D4CDF89}">
-  <dimension ref="A3:N5"/>
+  <dimension ref="A3:L5"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView zoomScale="150" workbookViewId="0">
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="25.33203125" customWidth="1"/>
-    <col min="12" max="12" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B3" s="1">
         <v>1</v>
       </c>
@@ -4271,20 +5461,14 @@
         <v>100000</v>
       </c>
       <c r="H3" s="1">
-        <v>500000</v>
-      </c>
-      <c r="I3" s="1">
         <v>1000000</v>
       </c>
-      <c r="J3" s="1">
-        <v>2000000</v>
-      </c>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
-      <c r="M3" s="1"/>
-      <c r="N3" s="1"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -4307,27 +5491,21 @@
         <v>12.23</v>
       </c>
       <c r="H4">
-        <v>60.65</v>
-      </c>
-      <c r="I4">
-        <v>121.24</v>
-      </c>
-      <c r="J4">
-        <v>241.99</v>
+        <v>120.81</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>1</v>
       </c>
       <c r="B5">
-        <v>0.09</v>
+        <v>0.11</v>
       </c>
       <c r="C5">
         <v>0.11</v>
       </c>
       <c r="D5">
-        <v>0.12</v>
+        <v>0.11</v>
       </c>
       <c r="E5">
         <v>0.23</v>
@@ -4336,16 +5514,110 @@
         <v>1.31</v>
       </c>
       <c r="G5">
-        <v>11.98</v>
+        <v>12.1</v>
       </c>
       <c r="H5">
-        <v>59.4</v>
-      </c>
-      <c r="I5">
-        <v>119.28</v>
-      </c>
-      <c r="J5">
-        <v>237.81</v>
+        <v>118.93</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{832F9567-5372-FC45-867D-7249C5F9991D}">
+  <dimension ref="A3:L5"/>
+  <sheetViews>
+    <sheetView zoomScale="150" workbookViewId="0">
+      <selection activeCell="E42" sqref="E42"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="25.33203125" customWidth="1"/>
+    <col min="10" max="10" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B3" s="1">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1">
+        <v>10</v>
+      </c>
+      <c r="D3" s="1">
+        <v>100</v>
+      </c>
+      <c r="E3" s="1">
+        <v>1000</v>
+      </c>
+      <c r="F3" s="1">
+        <v>10000</v>
+      </c>
+      <c r="G3" s="1">
+        <v>100000</v>
+      </c>
+      <c r="H3" s="1">
+        <v>1000000</v>
+      </c>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4">
+        <v>0.05</v>
+      </c>
+      <c r="C4">
+        <v>0.05</v>
+      </c>
+      <c r="D4">
+        <v>0.09</v>
+      </c>
+      <c r="E4">
+        <v>0.44</v>
+      </c>
+      <c r="F4">
+        <v>3.75</v>
+      </c>
+      <c r="G4">
+        <v>37.159999999999997</v>
+      </c>
+      <c r="H4">
+        <v>373.72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>0.12</v>
+      </c>
+      <c r="C5">
+        <v>0.12</v>
+      </c>
+      <c r="D5">
+        <v>0.16</v>
+      </c>
+      <c r="E5">
+        <v>0.48</v>
+      </c>
+      <c r="F5">
+        <v>3.88</v>
+      </c>
+      <c r="G5">
+        <v>38.03</v>
+      </c>
+      <c r="H5">
+        <v>375.77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Documented metanorma benchmarking results
</commit_message>
<xml_diff>
--- a/results/raw/results.xlsx
+++ b/results/raw/results.xlsx
@@ -1,71 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maxirmx/Projects/tebako-benchmarking/results/raw/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\8.Projects\tebako-benchmarking\results\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{368B570A-917E-234B-BB10-59EB06E74044}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5332CBAE-56B3-4B35-A005-7FCF922FF79E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="26380" activeTab="4" xr2:uid="{CC4E95A0-18F8-C345-87FB-74ABA326F855}"/>
+    <workbookView xWindow="3800" yWindow="2480" windowWidth="32730" windowHeight="18520" activeTab="4" xr2:uid="{CC4E95A0-18F8-C345-87FB-74ABA326F855}"/>
   </bookViews>
   <sheets>
     <sheet name="Simple script" sheetId="1" r:id="rId1"/>
     <sheet name="coradoc gem" sheetId="2" r:id="rId2"/>
     <sheet name="emf2svg gem" sheetId="3" r:id="rId3"/>
     <sheet name="vectory gem" sheetId="4" r:id="rId4"/>
-    <sheet name="vectory gem (2)" sheetId="5" r:id="rId5"/>
+    <sheet name="metanorma" sheetId="5" r:id="rId5"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">'vectory gem (2)'!$A$4</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">'vectory gem (2)'!$A$5</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">'vectory gem (2)'!$A$4</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">'vectory gem (2)'!$A$5</definedName>
-    <definedName name="_xlchart.v1.12" hidden="1">'vectory gem (2)'!$B$3:$H$3</definedName>
-    <definedName name="_xlchart.v1.13" hidden="1">'vectory gem (2)'!$B$4:$H$4</definedName>
-    <definedName name="_xlchart.v1.14" hidden="1">'vectory gem (2)'!$B$5:$H$5</definedName>
-    <definedName name="_xlchart.v1.15" hidden="1">'vectory gem (2)'!$A$4</definedName>
-    <definedName name="_xlchart.v1.16" hidden="1">'vectory gem (2)'!$A$5</definedName>
-    <definedName name="_xlchart.v1.17" hidden="1">'vectory gem (2)'!$B$3:$H$3</definedName>
-    <definedName name="_xlchart.v1.18" hidden="1">'vectory gem (2)'!$B$4:$H$4</definedName>
-    <definedName name="_xlchart.v1.19" hidden="1">'vectory gem (2)'!$B$5:$H$5</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">'vectory gem (2)'!$B$3:$H$3</definedName>
-    <definedName name="_xlchart.v1.20" hidden="1">'vectory gem (2)'!$A$4</definedName>
-    <definedName name="_xlchart.v1.21" hidden="1">'vectory gem (2)'!$A$5</definedName>
-    <definedName name="_xlchart.v1.22" hidden="1">'vectory gem (2)'!$B$3:$H$3</definedName>
-    <definedName name="_xlchart.v1.23" hidden="1">'vectory gem (2)'!$B$4:$H$4</definedName>
-    <definedName name="_xlchart.v1.24" hidden="1">'vectory gem (2)'!$B$5:$H$5</definedName>
-    <definedName name="_xlchart.v1.25" hidden="1">'vectory gem (2)'!$A$4</definedName>
-    <definedName name="_xlchart.v1.26" hidden="1">'vectory gem (2)'!$A$5</definedName>
-    <definedName name="_xlchart.v1.27" hidden="1">'vectory gem (2)'!$B$3:$H$3</definedName>
-    <definedName name="_xlchart.v1.28" hidden="1">'vectory gem (2)'!$B$4:$H$4</definedName>
-    <definedName name="_xlchart.v1.29" hidden="1">'vectory gem (2)'!$B$5:$H$5</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">'vectory gem (2)'!$B$4:$H$4</definedName>
-    <definedName name="_xlchart.v1.30" hidden="1">'vectory gem (2)'!$A$4</definedName>
-    <definedName name="_xlchart.v1.31" hidden="1">'vectory gem (2)'!$A$5</definedName>
-    <definedName name="_xlchart.v1.32" hidden="1">'vectory gem (2)'!$B$3:$H$3</definedName>
-    <definedName name="_xlchart.v1.33" hidden="1">'vectory gem (2)'!$B$4:$H$4</definedName>
-    <definedName name="_xlchart.v1.34" hidden="1">'vectory gem (2)'!$B$5:$H$5</definedName>
-    <definedName name="_xlchart.v1.35" hidden="1">'vectory gem (2)'!$A$4</definedName>
-    <definedName name="_xlchart.v1.36" hidden="1">'vectory gem (2)'!$A$5</definedName>
-    <definedName name="_xlchart.v1.37" hidden="1">'vectory gem (2)'!$B$3:$H$3</definedName>
-    <definedName name="_xlchart.v1.38" hidden="1">'vectory gem (2)'!$B$4:$H$4</definedName>
-    <definedName name="_xlchart.v1.39" hidden="1">'vectory gem (2)'!$B$5:$H$5</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">'vectory gem (2)'!$B$5:$H$5</definedName>
-    <definedName name="_xlchart.v1.40" hidden="1">'vectory gem (2)'!$A$4</definedName>
-    <definedName name="_xlchart.v1.41" hidden="1">'vectory gem (2)'!$A$5</definedName>
-    <definedName name="_xlchart.v1.42" hidden="1">'vectory gem (2)'!$B$3:$H$3</definedName>
-    <definedName name="_xlchart.v1.43" hidden="1">'vectory gem (2)'!$B$4:$H$4</definedName>
-    <definedName name="_xlchart.v1.44" hidden="1">'vectory gem (2)'!$B$5:$H$5</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">'vectory gem (2)'!$A$4</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">'vectory gem (2)'!$A$5</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">'vectory gem (2)'!$B$3:$H$3</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">'vectory gem (2)'!$B$4:$H$4</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">'vectory gem (2)'!$B$5:$H$5</definedName>
-  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -87,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="11">
   <si>
     <t xml:space="preserve">Plain Ruby </t>
   </si>
@@ -114,6 +67,12 @@
   </si>
   <si>
     <t>iho</t>
+  </si>
+  <si>
+    <t>Utility commands</t>
+  </si>
+  <si>
+    <t>Metanorma site generate</t>
   </si>
 </sst>
 </file>
@@ -149,12 +108,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -172,7 +140,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="ru-RU"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -234,7 +202,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-RU"/>
+          <a:endParaRPr lang="ru-RU"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -561,7 +529,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-RU"/>
+              <a:endParaRPr lang="ru-RU"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -599,7 +567,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-RU"/>
+            <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1858498064"/>
@@ -682,7 +650,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-RU"/>
+              <a:endParaRPr lang="ru-RU"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -714,7 +682,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-RU"/>
+            <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="521009296"/>
@@ -756,7 +724,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-RU"/>
+            <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
       </c:dTable>
@@ -801,7 +769,7 @@
       <a:pPr>
         <a:defRPr sz="1400"/>
       </a:pPr>
-      <a:endParaRPr lang="en-RU"/>
+      <a:endParaRPr lang="ru-RU"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -815,7 +783,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="ru-RU"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -877,7 +845,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-RU"/>
+          <a:endParaRPr lang="ru-RU"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1168,7 +1136,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-RU"/>
+              <a:endParaRPr lang="ru-RU"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1206,7 +1174,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-RU"/>
+            <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1858498064"/>
@@ -1289,7 +1257,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-RU"/>
+              <a:endParaRPr lang="ru-RU"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1321,7 +1289,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-RU"/>
+            <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="521009296"/>
@@ -1363,7 +1331,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-RU"/>
+            <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
       </c:dTable>
@@ -1408,7 +1376,7 @@
       <a:pPr>
         <a:defRPr sz="1400"/>
       </a:pPr>
-      <a:endParaRPr lang="en-RU"/>
+      <a:endParaRPr lang="ru-RU"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1422,7 +1390,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="ru-RU"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1484,7 +1452,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-RU"/>
+          <a:endParaRPr lang="ru-RU"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1775,7 +1743,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-RU"/>
+              <a:endParaRPr lang="ru-RU"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1813,7 +1781,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-RU"/>
+            <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1858498064"/>
@@ -1896,7 +1864,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-RU"/>
+              <a:endParaRPr lang="ru-RU"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1928,7 +1896,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-RU"/>
+            <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="521009296"/>
@@ -1970,7 +1938,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-RU"/>
+            <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
       </c:dTable>
@@ -2015,7 +1983,7 @@
       <a:pPr>
         <a:defRPr sz="1400"/>
       </a:pPr>
-      <a:endParaRPr lang="en-RU"/>
+      <a:endParaRPr lang="ru-RU"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2029,7 +1997,7 @@
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="ru-RU"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2091,7 +2059,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-RU"/>
+          <a:endParaRPr lang="ru-RU"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -2382,7 +2350,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-RU"/>
+              <a:endParaRPr lang="ru-RU"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -2420,7 +2388,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-RU"/>
+            <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1858498064"/>
@@ -2503,7 +2471,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-RU"/>
+              <a:endParaRPr lang="ru-RU"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -2535,7 +2503,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-RU"/>
+            <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="521009296"/>
@@ -2577,7 +2545,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-RU"/>
+            <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
       </c:dTable>
@@ -2622,7 +2590,7 @@
       <a:pPr>
         <a:defRPr sz="1400"/>
       </a:pPr>
-      <a:endParaRPr lang="en-RU"/>
+      <a:endParaRPr lang="ru-RU"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2636,7 +2604,7 @@
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="ru-RU"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2668,7 +2636,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-GB"/>
-              <a:t> Benchmarking for vectory gem</a:t>
+              <a:t> Benchmarking for metanorma</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -2698,7 +2666,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-RU"/>
+          <a:endParaRPr lang="ru-RU"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -2714,7 +2682,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'vectory gem (2)'!$A$4</c:f>
+              <c:f>metanorma!$A$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2734,37 +2702,47 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
-            <c:strRef>
-              <c:f>'vectory gem (2)'!$B$3:$H$3</c:f>
-              <c:strCache>
+            <c:multiLvlStrRef>
+              <c:f>metanorma!$B$2:$H$3</c:f>
+              <c:multiLvlStrCache>
                 <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>help</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>version</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>ietf</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>ieee</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>iec</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>iho</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>iso</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>help</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>version</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>ietf</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>ieee</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>iec</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>iho</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>iso</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Utility commands</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Metanorma site generate</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'vectory gem (2)'!$B$4:$H$4</c:f>
+              <c:f>metanorma!$B$4:$H$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -2803,7 +2781,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'vectory gem (2)'!$A$5</c:f>
+              <c:f>metanorma!$A$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2823,37 +2801,47 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
-            <c:strRef>
-              <c:f>'vectory gem (2)'!$B$3:$H$3</c:f>
-              <c:strCache>
+            <c:multiLvlStrRef>
+              <c:f>metanorma!$B$2:$H$3</c:f>
+              <c:multiLvlStrCache>
                 <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>help</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>version</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>ietf</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>ieee</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>iec</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>iho</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>iso</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>help</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>version</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>ietf</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>ieee</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>iec</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>iho</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>iso</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Utility commands</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Metanorma site generate</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'vectory gem (2)'!$B$5:$H$5</c:f>
+              <c:f>metanorma!$B$5:$H$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -2957,7 +2945,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-RU"/>
+              <a:endParaRPr lang="ru-RU"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -2995,7 +2983,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-RU"/>
+            <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1858498064"/>
@@ -3077,7 +3065,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-RU"/>
+              <a:endParaRPr lang="ru-RU"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -3109,7 +3097,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-RU"/>
+            <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="521009296"/>
@@ -3125,10 +3113,7 @@
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
+              <a:schemeClr val="accent1"/>
             </a:solidFill>
             <a:round/>
           </a:ln>
@@ -3151,7 +3136,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-RU"/>
+            <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
       </c:dTable>
@@ -3196,7 +3181,7 @@
       <a:pPr>
         <a:defRPr sz="1400"/>
       </a:pPr>
-      <a:endParaRPr lang="en-RU"/>
+      <a:endParaRPr lang="ru-RU"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -6136,9 +6121,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -6176,7 +6161,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -6282,7 +6267,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -6438,14 +6423,14 @@
       <selection activeCell="C57" sqref="C57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="25.33203125" customWidth="1"/>
     <col min="10" max="10" width="11.1640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B3" s="1">
         <v>1</v>
       </c>
@@ -6478,7 +6463,7 @@
       </c>
       <c r="L3" s="1"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -6513,7 +6498,7 @@
         <v>1759.48</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -6562,14 +6547,14 @@
       <selection activeCell="C62" sqref="C62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="25.33203125" customWidth="1"/>
     <col min="11" max="11" width="11.1640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B3" s="1">
         <v>1</v>
       </c>
@@ -6597,7 +6582,7 @@
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -6623,7 +6608,7 @@
         <v>1643.93</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -6663,14 +6648,14 @@
       <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="25.33203125" customWidth="1"/>
     <col min="10" max="10" width="11.1640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B3" s="1">
         <v>1</v>
       </c>
@@ -6697,7 +6682,7 @@
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -6723,7 +6708,7 @@
         <v>120.81</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -6763,14 +6748,14 @@
       <selection activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="25.33203125" customWidth="1"/>
     <col min="10" max="10" width="11.1640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B3" s="1">
         <v>1</v>
       </c>
@@ -6797,7 +6782,7 @@
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -6823,7 +6808,7 @@
         <v>373.72</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -6857,39 +6842,52 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1430684C-BF99-A647-897C-5D67FE9DCC5C}">
-  <dimension ref="A3:L5"/>
+  <dimension ref="A2:L5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="150" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="R53" sqref="R53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="25.33203125" customWidth="1"/>
     <col min="10" max="10" width="11.1640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B3" s="1" t="s">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="B2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="B3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="G3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="H3" s="4" t="s">
         <v>7</v>
       </c>
       <c r="I3" s="1"/>
@@ -6897,69 +6895,73 @@
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>0</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="2">
         <v>1.92</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="2">
         <v>2.92</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="2">
         <f>7.77+2.68</f>
         <v>10.45</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="2">
         <f>18.65+3.12</f>
         <v>21.77</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="2">
         <f>56.74+4.59</f>
         <v>61.33</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="2">
         <f>63.74+6.94</f>
         <v>70.680000000000007</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="2">
         <f>230.67+18.23</f>
         <v>248.89999999999998</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>1</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="2">
         <v>3</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="2">
         <v>4.5199999999999996</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="2">
         <f>11.91+1.6</f>
         <v>13.51</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="2">
         <f>21.65+2.04</f>
         <v>23.689999999999998</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="2">
         <f>60.85+3.29</f>
         <v>64.14</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="2">
         <f>68.44+6.24</f>
         <v>74.679999999999993</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="2">
         <f>234.95+17.28</f>
         <v>252.23</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:H2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Finalized benchmarking results (#6)
</commit_message>
<xml_diff>
--- a/results/raw/results.xlsx
+++ b/results/raw/results.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maxirmx/Projects/tebako-benchmarking/results/raw/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\8.Projects\tebako-benchmarking\results\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3D9FCCE-AED9-944D-B8AA-1458DDDB086D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19EEA05F-D982-4CC2-A697-01780FA89EED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="26380" xr2:uid="{CC4E95A0-18F8-C345-87FB-74ABA326F855}"/>
+    <workbookView xWindow="3800" yWindow="2480" windowWidth="32730" windowHeight="18520" activeTab="4" xr2:uid="{CC4E95A0-18F8-C345-87FB-74ABA326F855}"/>
   </bookViews>
   <sheets>
     <sheet name="Simple script" sheetId="1" r:id="rId1"/>
     <sheet name="coradoc gem" sheetId="2" r:id="rId2"/>
     <sheet name="emf2svg gem" sheetId="3" r:id="rId3"/>
     <sheet name="vectory gem" sheetId="4" r:id="rId4"/>
+    <sheet name="metanorma" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,12 +40,39 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="11">
   <si>
     <t xml:space="preserve">Plain Ruby </t>
   </si>
   <si>
     <t>Tebako package</t>
+  </si>
+  <si>
+    <t>help</t>
+  </si>
+  <si>
+    <t>version</t>
+  </si>
+  <si>
+    <t>ietf</t>
+  </si>
+  <si>
+    <t>ieee</t>
+  </si>
+  <si>
+    <t>iec</t>
+  </si>
+  <si>
+    <t>iso</t>
+  </si>
+  <si>
+    <t>iho</t>
+  </si>
+  <si>
+    <t>Utility commands</t>
+  </si>
+  <si>
+    <t>Metanorma site generate</t>
   </si>
 </sst>
 </file>
@@ -80,12 +108,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -103,7 +140,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="ru-RU"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -165,7 +202,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-RU"/>
+          <a:endParaRPr lang="ru-RU"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -492,7 +529,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-RU"/>
+              <a:endParaRPr lang="ru-RU"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -530,7 +567,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-RU"/>
+            <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1858498064"/>
@@ -613,7 +650,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-RU"/>
+              <a:endParaRPr lang="ru-RU"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -645,7 +682,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-RU"/>
+            <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="521009296"/>
@@ -687,7 +724,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-RU"/>
+            <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
       </c:dTable>
@@ -732,7 +769,7 @@
       <a:pPr>
         <a:defRPr sz="1400"/>
       </a:pPr>
-      <a:endParaRPr lang="en-RU"/>
+      <a:endParaRPr lang="ru-RU"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -746,7 +783,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="ru-RU"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -808,7 +845,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-RU"/>
+          <a:endParaRPr lang="ru-RU"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1099,7 +1136,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-RU"/>
+              <a:endParaRPr lang="ru-RU"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1137,7 +1174,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-RU"/>
+            <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1858498064"/>
@@ -1220,7 +1257,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-RU"/>
+              <a:endParaRPr lang="ru-RU"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1252,7 +1289,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-RU"/>
+            <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="521009296"/>
@@ -1294,7 +1331,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-RU"/>
+            <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
       </c:dTable>
@@ -1339,7 +1376,7 @@
       <a:pPr>
         <a:defRPr sz="1400"/>
       </a:pPr>
-      <a:endParaRPr lang="en-RU"/>
+      <a:endParaRPr lang="ru-RU"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1353,7 +1390,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="ru-RU"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1415,7 +1452,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-RU"/>
+          <a:endParaRPr lang="ru-RU"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1706,7 +1743,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-RU"/>
+              <a:endParaRPr lang="ru-RU"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1744,7 +1781,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-RU"/>
+            <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1858498064"/>
@@ -1827,7 +1864,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-RU"/>
+              <a:endParaRPr lang="ru-RU"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1859,7 +1896,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-RU"/>
+            <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="521009296"/>
@@ -1901,7 +1938,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-RU"/>
+            <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
       </c:dTable>
@@ -1946,7 +1983,7 @@
       <a:pPr>
         <a:defRPr sz="1400"/>
       </a:pPr>
-      <a:endParaRPr lang="en-RU"/>
+      <a:endParaRPr lang="ru-RU"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1960,7 +1997,7 @@
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="ru-RU"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2022,7 +2059,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-RU"/>
+          <a:endParaRPr lang="ru-RU"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -2313,7 +2350,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-RU"/>
+              <a:endParaRPr lang="ru-RU"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -2351,7 +2388,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-RU"/>
+            <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1858498064"/>
@@ -2434,7 +2471,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-RU"/>
+              <a:endParaRPr lang="ru-RU"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -2466,7 +2503,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-RU"/>
+            <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="521009296"/>
@@ -2508,7 +2545,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-RU"/>
+            <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
       </c:dTable>
@@ -2553,7 +2590,598 @@
       <a:pPr>
         <a:defRPr sz="1400"/>
       </a:pPr>
-      <a:endParaRPr lang="en-RU"/>
+      <a:endParaRPr lang="ru-RU"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="ru-RU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1680" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t> Benchmarking for metanorma</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1680" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ru-RU"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>metanorma!$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Plain Ruby </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>metanorma!$B$2:$H$3</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="7"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>help</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>version</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>ietf</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>ieee</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>iec</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>iho</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>iso</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Utility commands</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Metanorma site generate</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>metanorma!$B$4:$H$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1.92</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.92</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10.45</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>21.77</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>61.33</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>71.679999999999993</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>248.89999999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-4485-F94D-9367-75C2FE92B452}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>metanorma!$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Tebako package</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>metanorma!$B$2:$H$3</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="7"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>help</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>version</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>ietf</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>ieee</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>iec</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>iho</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>iso</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Utility commands</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Metanorma site generate</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>metanorma!$B$5:$H$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.5199999999999996</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>13.51</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>23.689999999999998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>64.14</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>74.679999999999993</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>252.23</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-4485-F94D-9367-75C2FE92B452}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="521009296"/>
+        <c:axId val="1858498064"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="521009296"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Number of repetitions</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="ru-RU"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1858498064"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1858498064"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Execution time (user + sys), seconds</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="ru-RU"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="521009296"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:dTable>
+        <c:showHorzBorder val="1"/>
+        <c:showVertBorder val="1"/>
+        <c:showOutline val="1"/>
+        <c:showKeys val="1"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr rtl="0">
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+      </c:dTable>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1400"/>
+      </a:pPr>
+      <a:endParaRPr lang="ru-RU"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2724,6 +3352,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
@@ -4234,6 +4902,509 @@
 </file>
 
 <file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -4906,10 +6077,53 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>806450</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{43F87314-29C0-4249-87AA-8763D45EBD3A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -4947,7 +6161,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -5053,7 +6267,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -5205,18 +6419,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{011826E9-9A44-C042-A061-04C93FF74651}">
   <dimension ref="A3:L5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C57" sqref="C57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="25.33203125" customWidth="1"/>
     <col min="10" max="10" width="11.1640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B3" s="1">
         <v>1</v>
       </c>
@@ -5249,7 +6463,7 @@
       </c>
       <c r="L3" s="1"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -5284,7 +6498,7 @@
         <v>1759.48</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -5333,14 +6547,14 @@
       <selection activeCell="C62" sqref="C62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="25.33203125" customWidth="1"/>
     <col min="11" max="11" width="11.1640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B3" s="1">
         <v>1</v>
       </c>
@@ -5368,7 +6582,7 @@
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -5394,7 +6608,7 @@
         <v>1643.93</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -5434,14 +6648,14 @@
       <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="25.33203125" customWidth="1"/>
     <col min="10" max="10" width="11.1640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B3" s="1">
         <v>1</v>
       </c>
@@ -5468,7 +6682,7 @@
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -5494,7 +6708,7 @@
         <v>120.81</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -5534,14 +6748,14 @@
       <selection activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="25.33203125" customWidth="1"/>
     <col min="10" max="10" width="11.1640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B3" s="1">
         <v>1</v>
       </c>
@@ -5568,7 +6782,7 @@
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -5594,7 +6808,7 @@
         <v>373.72</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -5624,4 +6838,131 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1430684C-BF99-A647-897C-5D67FE9DCC5C}">
+  <dimension ref="A2:L5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="25.33203125" customWidth="1"/>
+    <col min="10" max="10" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="B2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="B3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="2">
+        <v>1.92</v>
+      </c>
+      <c r="C4" s="2">
+        <v>2.92</v>
+      </c>
+      <c r="D4" s="2">
+        <f>7.77+2.68</f>
+        <v>10.45</v>
+      </c>
+      <c r="E4" s="2">
+        <f>18.65+3.12</f>
+        <v>21.77</v>
+      </c>
+      <c r="F4" s="2">
+        <f>56.74+4.59</f>
+        <v>61.33</v>
+      </c>
+      <c r="G4" s="2">
+        <f>64.74+6.94</f>
+        <v>71.679999999999993</v>
+      </c>
+      <c r="H4" s="2">
+        <f>230.67+18.23</f>
+        <v>248.89999999999998</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="2">
+        <v>3</v>
+      </c>
+      <c r="C5" s="2">
+        <v>4.5199999999999996</v>
+      </c>
+      <c r="D5" s="2">
+        <f>11.91+1.6</f>
+        <v>13.51</v>
+      </c>
+      <c r="E5" s="2">
+        <f>21.65+2.04</f>
+        <v>23.689999999999998</v>
+      </c>
+      <c r="F5" s="2">
+        <f>60.85+3.29</f>
+        <v>64.14</v>
+      </c>
+      <c r="G5" s="2">
+        <f>68.44+6.24</f>
+        <v>74.679999999999993</v>
+      </c>
+      <c r="H5" s="2">
+        <f>234.95+17.28</f>
+        <v>252.23</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:H2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>